<commit_message>
added Spyder project file
</commit_message>
<xml_diff>
--- a/oraculo_prototype/tests/test_test_live_2_@CorbeauNews_snips_output.xlsx
+++ b/oraculo_prototype/tests/test_test_live_2_@CorbeauNews_snips_output.xlsx
@@ -1214,10 +1214,82 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>2022-09-13T00:02:09.000Z</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Centrafrique : la plateforme des jeunes leaders de l’opposition appelle ses points focaux provinciaux à descendre à Bangui
+...
+corbeaunews-centrafrique.org
+Centrafrique : la plateforme des jeunes leaders de l’opposition appelle ses points focaux provinc...
+1
+2
+3</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://twitter.com/CorbeauNews/status/1569476491833925634</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Central African Republic the platform of young opposition leaders calls on its provincial focal points to go to Bangui ... corbeaunews-centrafrique.org Central African Republic the platform of young opposition leaders calls on its provincial focal... 1 2 3</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9856086684370484</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>['calls', 'calls']</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>['opposition leaders', 'opposition leaders']</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2022-09-13T00:02:09.000Z</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>['Central African Republic', 'Bangui', 'Central African Republic']</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>['Two']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>@CorbeauNews</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>2022-09-13T00:13:23.000Z</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>RCA : le rapprochement du chef rebelle Abakar Sabone au Président Touadera a-t-il échoué ?
 ...
@@ -1228,122 +1300,50 @@
 3</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>https://twitter.com/CorbeauNews/status/1569479318148972545</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>CAR Has the rapprochement between rebel leader Abakar Sabone and President Touadera failed ... corbeaunews-centrafrique.org CAR Has the rapprochement between rebel leader Abakar Sabone and President Touadera failed 2 2 3</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.9699547173882912</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>['Has', 'Abakar Sabone', 'org CAR', 'Abakar Sabone']</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>['President Touadera', 'President Touadera']</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>2022-09-13T00:13:23.000Z</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>['CAR', 'rapprochement', 'rapprochement']</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>['Two', '3']</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>@CorbeauNews</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2022-09-13T00:02:09.000Z</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Centrafrique : la plateforme des jeunes leaders de l’opposition appelle ses points focaux provinciaux à descendre à Bangui
-...
-corbeaunews-centrafrique.org
-Centrafrique : la plateforme des jeunes leaders de l’opposition appelle ses points focaux provinc...
-1
-2
-3</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>https://twitter.com/CorbeauNews/status/1569476491833925634</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Central African Republic the platform of young opposition leaders calls on its provincial focal points to go to Bangui ... corbeaunews-centrafrique.org Central African Republic the platform of young opposition leaders calls on its provincial focal... 1 2 3</t>
         </is>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9856086684370484</v>
+        <v>0.9699547173882912</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>['calls', 'calls']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['opposition leaders', 'opposition leaders']</t>
+          <t>['Has', 'Abakar Sabone', 'org CAR', 'Abakar Sabone']</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['President Touadera', 'President Touadera']</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2022-09-13T00:02:09.000Z</t>
+          <t>2022-09-13T00:13:23.000Z</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>['Central African Republic', 'Bangui', 'Central African Republic']</t>
+          <t>['CAR', 'rapprochement', 'rapprochement']</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>['Two']</t>
+          <t>['Two', '3']</t>
         </is>
       </c>
     </row>

</xml_diff>